<commit_message>
Final version without mistakes
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -22,20 +22,20 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Souvent, pour s’amuser, les hommes d’équipage
+    <t xml:space="preserve">Souvent, pour s’amuser, les hommes d’équipage,
 Prennent des albatros, vastes oiseaux des mers,
 Qui suivent, indolents compagnons de voyage,
 Le navire glissant sur les gouffres amers.
 À peine les ont-ils déposés sur les planches,
 Que ces rois de l'azur, maladroits et honteux,
-Laissent piteusement leurs grandes ailes blanches
+Laissent piteusement leurs grandes ailes blanches.
 Comme des avirons traîner à côté d'eux.
 Ce voyageur ailé, comme il est gauche et veule !
 Lui, naguère si beau, qu'il est comique et laid !
 L'un agace son bec avec un brûle-gueule,
 L'autre mime, en boitant, l'infirme qui volait !
-Le Poète est semblable au prince des nuées
-Qui hante la tempête et se rit de l'archer ;
+Le Poète est semblable au prince des nuées.
+Qui hante la tempête et se rit de l'archer;
 Exilé sur le sol au milieu des huées,
 Ses ailes de géant l'empêchent de marcher. </t>
   </si>
@@ -145,12 +145,15 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="62.62"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="256.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>